<commit_message>
sort index for AUC ranking
</commit_message>
<xml_diff>
--- a/plot_results/roc/auc_mean.xlsx
+++ b/plot_results/roc/auc_mean.xlsx
@@ -545,29 +545,29 @@
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>Cancer</t>
+          <t>CYP1A2</t>
         </is>
       </c>
       <c r="B4" t="n">
+        <v>5</v>
+      </c>
+      <c r="C4" t="n">
+        <v>6</v>
+      </c>
+      <c r="D4" t="n">
         <v>7</v>
-      </c>
-      <c r="C4" t="n">
-        <v>5</v>
-      </c>
-      <c r="D4" t="n">
-        <v>5</v>
       </c>
       <c r="E4" t="n">
         <v>8</v>
       </c>
       <c r="F4" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G4" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I4" t="n">
         <v>2</v>
@@ -576,29 +576,29 @@
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>CYP1A2</t>
+          <t>Cancer</t>
         </is>
       </c>
       <c r="B5" t="n">
+        <v>7</v>
+      </c>
+      <c r="C5" t="n">
         <v>5</v>
       </c>
-      <c r="C5" t="n">
-        <v>6</v>
-      </c>
       <c r="D5" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E5" t="n">
         <v>8</v>
       </c>
       <c r="F5" t="n">
+        <v>3</v>
+      </c>
+      <c r="G5" t="n">
+        <v>3</v>
+      </c>
+      <c r="H5" t="n">
         <v>1</v>
-      </c>
-      <c r="G5" t="n">
-        <v>4</v>
-      </c>
-      <c r="H5" t="n">
-        <v>2</v>
       </c>
       <c r="I5" t="n">
         <v>2</v>
@@ -607,11 +607,11 @@
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>hERG</t>
+          <t>HIV</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C6" t="n">
         <v>7</v>
@@ -620,7 +620,7 @@
         <v>8</v>
       </c>
       <c r="E6" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F6" t="n">
         <v>1</v>
@@ -638,26 +638,26 @@
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>HIV</t>
+          <t>Liver</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C7" t="n">
+        <v>5</v>
+      </c>
+      <c r="D7" t="n">
+        <v>6</v>
+      </c>
+      <c r="E7" t="n">
         <v>7</v>
-      </c>
-      <c r="D7" t="n">
-        <v>8</v>
-      </c>
-      <c r="E7" t="n">
-        <v>6</v>
       </c>
       <c r="F7" t="n">
         <v>1</v>
       </c>
       <c r="G7" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H7" t="n">
         <v>2</v>
@@ -669,26 +669,26 @@
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>Liver</t>
+          <t>hERG</t>
         </is>
       </c>
       <c r="B8" t="n">
+        <v>5</v>
+      </c>
+      <c r="C8" t="n">
+        <v>7</v>
+      </c>
+      <c r="D8" t="n">
         <v>8</v>
       </c>
-      <c r="C8" t="n">
+      <c r="E8" t="n">
         <v>5</v>
-      </c>
-      <c r="D8" t="n">
-        <v>6</v>
-      </c>
-      <c r="E8" t="n">
-        <v>7</v>
       </c>
       <c r="F8" t="n">
         <v>1</v>
       </c>
       <c r="G8" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H8" t="n">
         <v>2</v>

</xml_diff>